<commit_message>
Cleaned Team names and codes XLSX and CSV
</commit_message>
<xml_diff>
--- a/Raw_Data/NBA Team Names and codes.xlsx
+++ b/Raw_Data/NBA Team Names and codes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulf\OneDrive\Documents\bootcamp\project-one\Raw Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulf\OneDrive\Documents\bootcamp\project-one\Raw_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66A4EB88-C4A1-4DA1-B4B9-F4FDC6C24C5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94437BC0-71E8-4CDE-AA15-358AA207F349}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{597059BC-8037-4542-BBB6-66A90E5DA58E}"/>
   </bookViews>
@@ -33,74 +33,35 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Atl</t>
   </si>
   <si>
-    <t>Atlanta</t>
-  </si>
-  <si>
     <t>Bos</t>
   </si>
   <si>
-    <t>Boston</t>
-  </si>
-  <si>
-    <t>Cha</t>
-  </si>
-  <si>
-    <t>Charlotte</t>
-  </si>
-  <si>
     <t>Chi</t>
   </si>
   <si>
-    <t>Chicago</t>
-  </si>
-  <si>
     <t>Cle</t>
   </si>
   <si>
-    <t>Cleveland</t>
-  </si>
-  <si>
     <t>Dal</t>
   </si>
   <si>
-    <t>Dallas</t>
-  </si>
-  <si>
     <t>Den</t>
   </si>
   <si>
-    <t>Denver</t>
-  </si>
-  <si>
     <t>Det</t>
   </si>
   <si>
-    <t>Detroit</t>
-  </si>
-  <si>
-    <t>GS</t>
-  </si>
-  <si>
-    <t>Golden State</t>
-  </si>
-  <si>
     <t>Hou</t>
   </si>
   <si>
-    <t>Houston</t>
-  </si>
-  <si>
     <t>Ind</t>
   </si>
   <si>
-    <t>Indiana</t>
-  </si>
-  <si>
     <t>LAC</t>
   </si>
   <si>
@@ -116,122 +77,155 @@
     <t>Mem</t>
   </si>
   <si>
-    <t>Memphis</t>
-  </si>
-  <si>
     <t>Mia</t>
   </si>
   <si>
-    <t>Miami</t>
-  </si>
-  <si>
     <t>Mil</t>
   </si>
   <si>
-    <t>Milwaukee</t>
-  </si>
-  <si>
     <t>Min</t>
   </si>
   <si>
-    <t>Minnesota</t>
-  </si>
-  <si>
-    <t>NJ</t>
-  </si>
-  <si>
-    <t>New Jersey</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>New Orleans</t>
-  </si>
-  <si>
-    <t>NY</t>
-  </si>
-  <si>
-    <t>New York</t>
-  </si>
-  <si>
     <t>Orl</t>
   </si>
   <si>
-    <t>Orlando</t>
-  </si>
-  <si>
     <t>Phi</t>
   </si>
   <si>
-    <t>Philadelphia</t>
-  </si>
-  <si>
-    <t>Phx</t>
-  </si>
-  <si>
-    <t>Phoenix</t>
-  </si>
-  <si>
     <t>Por</t>
   </si>
   <si>
-    <t>Portland</t>
-  </si>
-  <si>
-    <t>SA</t>
-  </si>
-  <si>
-    <t>San Antonio</t>
-  </si>
-  <si>
     <t>Sac</t>
   </si>
   <si>
-    <t>Sacramento</t>
-  </si>
-  <si>
-    <t>Sea</t>
-  </si>
-  <si>
-    <t>Seattle</t>
-  </si>
-  <si>
     <t>Tor</t>
   </si>
   <si>
-    <t>Toronto</t>
-  </si>
-  <si>
-    <t>Uth</t>
-  </si>
-  <si>
-    <t>Utah</t>
-  </si>
-  <si>
-    <t>Van</t>
-  </si>
-  <si>
-    <t>Vancouver</t>
-  </si>
-  <si>
-    <t>Wsh</t>
-  </si>
-  <si>
-    <t>Washington</t>
-  </si>
-  <si>
     <t>Team Code</t>
   </si>
   <si>
     <t>Team Name</t>
+  </si>
+  <si>
+    <t>Atlanta Hawks</t>
+  </si>
+  <si>
+    <t>Boston Celtics</t>
+  </si>
+  <si>
+    <t>Brk</t>
+  </si>
+  <si>
+    <t>Brooklyn Nets</t>
+  </si>
+  <si>
+    <t>Chicago Bulls</t>
+  </si>
+  <si>
+    <t>Cleveland Cavaliers</t>
+  </si>
+  <si>
+    <t>Cho</t>
+  </si>
+  <si>
+    <t>Charlotte Hornets</t>
+  </si>
+  <si>
+    <t>Dallas Mavericks</t>
+  </si>
+  <si>
+    <t>Denver Nuggets</t>
+  </si>
+  <si>
+    <t>Detroit Pistons</t>
+  </si>
+  <si>
+    <t>Golden State Warriors</t>
+  </si>
+  <si>
+    <t>Houston Rockets</t>
+  </si>
+  <si>
+    <t>Indiana Pacers</t>
+  </si>
+  <si>
+    <t>Memphis Grizzlies</t>
+  </si>
+  <si>
+    <t>Miami Heat</t>
+  </si>
+  <si>
+    <t>Milwaukee Bucks</t>
+  </si>
+  <si>
+    <t>Minnesota Timberwolves</t>
+  </si>
+  <si>
+    <t>New Orleans Pelicans</t>
+  </si>
+  <si>
+    <t>New York Knicks</t>
+  </si>
+  <si>
+    <t>Nop</t>
+  </si>
+  <si>
+    <t>Nyk</t>
+  </si>
+  <si>
+    <t>Okc</t>
+  </si>
+  <si>
+    <t>Oklahoma City Thunder</t>
+  </si>
+  <si>
+    <t>Orlando Magic</t>
+  </si>
+  <si>
+    <t>Philadelphia 76ers</t>
+  </si>
+  <si>
+    <t>Phoenix Suns</t>
+  </si>
+  <si>
+    <t>Portland Trail Blazers</t>
+  </si>
+  <si>
+    <t>Sacramento Kings</t>
+  </si>
+  <si>
+    <t>Sas</t>
+  </si>
+  <si>
+    <t>San Antonio Spurs</t>
+  </si>
+  <si>
+    <t>Toronto Raptors</t>
+  </si>
+  <si>
+    <t>Uta</t>
+  </si>
+  <si>
+    <t>Utah Jazz</t>
+  </si>
+  <si>
+    <t>Was</t>
+  </si>
+  <si>
+    <t>Washington Wizards</t>
+  </si>
+  <si>
+    <t>Gsw</t>
+  </si>
+  <si>
+    <t>Pho</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,7 +234,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -281,9 +282,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -600,272 +602,265 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEB53C83-DBF1-4E45-BCD9-918D91D75284}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="16" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="B7" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B8" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="B9" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B10" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="B12" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B13" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="1" t="s">
+    </row>
+    <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="B16" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B17" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="B18" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B19" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="B23" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B24" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="B26" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B28" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="2" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>